<commit_message>
Fix: add afterDataChange and remove duplicate variable declarations
Changed files:
- function/simulation.js: added afterDataChange function and removed duplicate variable/function declarations causing redeclaration errors
</commit_message>
<xml_diff>
--- a/original-excel-sources/budget_jeanre.xlsx
+++ b/original-excel-sources/budget_jeanre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jay/GIT-Repos-Personal/ftrack/original-excel-sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8279978-2666-9C49-9FF6-4916B1D042F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD40F6A-CE18-C74C-8B10-EAEA73A320F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-68800" yWindow="-10980" windowWidth="68800" windowHeight="28300" xr2:uid="{F25DD163-696E-F842-A897-5E899A2812A7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="86">
   <si>
     <t>Jeanre Transactional</t>
   </si>
@@ -221,126 +221,12 @@
     <t>econo</t>
   </si>
   <si>
-    <t>total</t>
-  </si>
-  <si>
-    <t>game</t>
-  </si>
-  <si>
-    <t>dis chem</t>
-  </si>
-  <si>
-    <t>food lovers</t>
-  </si>
-  <si>
-    <t>Leftover</t>
-  </si>
-  <si>
-    <t>jay main</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bulk meat </t>
-  </si>
-  <si>
-    <t>shoprite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">food lovers </t>
-  </si>
-  <si>
-    <t xml:space="preserve">westpack </t>
-  </si>
-  <si>
-    <t>airtime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kfc </t>
-  </si>
-  <si>
     <t>fuel</t>
   </si>
   <si>
-    <t>checkers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dis chem </t>
-  </si>
-  <si>
-    <t>checkers - mother weekend</t>
-  </si>
-  <si>
-    <t>fuel mother weekend</t>
-  </si>
-  <si>
-    <t>garage mother weekend</t>
-  </si>
-  <si>
-    <t>spar mother weekend</t>
-  </si>
-  <si>
-    <t>claim from BCL for april</t>
-  </si>
-  <si>
-    <t>B credit card</t>
-  </si>
-  <si>
     <t>Game</t>
   </si>
   <si>
-    <t>vision meat</t>
-  </si>
-  <si>
-    <t>3700 from jay</t>
-  </si>
-  <si>
-    <t>4500 from B credit card</t>
-  </si>
-  <si>
-    <t>8200 budget total</t>
-  </si>
-  <si>
-    <t>1384 over budget</t>
-  </si>
-  <si>
-    <t>1873 from b credit card</t>
-  </si>
-  <si>
-    <t>7711 from jay main</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2627 needed from b credit card </t>
-  </si>
-  <si>
-    <t xml:space="preserve">I have </t>
-  </si>
-  <si>
-    <t>I am getting</t>
-  </si>
-  <si>
-    <t>municipal account</t>
-  </si>
-  <si>
-    <t>medical</t>
-  </si>
-  <si>
-    <t>shortfall</t>
-  </si>
-  <si>
-    <t>gap between these two is because of the leftover from the food budget</t>
-  </si>
-  <si>
-    <t>1015 for mother weekend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from bernice credit card. </t>
-  </si>
-  <si>
-    <t>i can pay now</t>
-  </si>
-  <si>
-    <t xml:space="preserve">extra next month: </t>
-  </si>
-  <si>
     <t>no retain</t>
   </si>
   <si>
@@ -351,6 +237,63 @@
   </si>
   <si>
     <t>Child Fund</t>
+  </si>
+  <si>
+    <t>Macbook</t>
+  </si>
+  <si>
+    <t>Delhi Delicious</t>
+  </si>
+  <si>
+    <t>midtown</t>
+  </si>
+  <si>
+    <t>hair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniel in </t>
+  </si>
+  <si>
+    <t>herbs and spices</t>
+  </si>
+  <si>
+    <t>takealot</t>
+  </si>
+  <si>
+    <t>kfc</t>
+  </si>
+  <si>
+    <t>bestmed</t>
+  </si>
+  <si>
+    <t>dischem</t>
+  </si>
+  <si>
+    <t>mcd</t>
+  </si>
+  <si>
+    <t>Municipal ac</t>
+  </si>
+  <si>
+    <t>Psych</t>
+  </si>
+  <si>
+    <t>RAm for mac</t>
+  </si>
+  <si>
+    <t>pathcare</t>
+  </si>
+  <si>
+    <t>grandparents</t>
+  </si>
+  <si>
+    <t>NM</t>
+  </si>
+  <si>
+    <t>emergency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from wealth? </t>
   </si>
 </sst>
 </file>
@@ -360,7 +303,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -475,20 +418,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF006100"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C5700"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="16"/>
       <color rgb="FF00B0F0"/>
@@ -502,8 +431,37 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -534,18 +492,8 @@
         <bgColor theme="0" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -593,21 +541,6 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
@@ -617,41 +550,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -669,7 +572,7 @@
     <xf numFmtId="44" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -690,42 +593,40 @@
     <xf numFmtId="44" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="14" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="15" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="1"/>
-    <xf numFmtId="44" fontId="18" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="18" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="19" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="19" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="16" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="16" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="17" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="48">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -765,7 +666,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color auto="1"/>
+        <color theme="1"/>
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
@@ -773,7 +674,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -813,7 +714,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color auto="1"/>
+        <color theme="1"/>
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
@@ -821,7 +722,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -861,7 +762,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color auto="1"/>
+        <color theme="1"/>
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
@@ -869,7 +770,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -909,7 +810,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color auto="1"/>
+        <color theme="1"/>
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
@@ -917,7 +818,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -957,7 +858,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color auto="1"/>
+        <color theme="1"/>
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
@@ -965,7 +866,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -990,318 +891,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1352,7 +941,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color auto="1"/>
+        <color theme="1"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1361,9 +950,19 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1412,7 +1011,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color auto="1"/>
+        <color theme="1"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1421,9 +1020,19 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1472,7 +1081,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color auto="1"/>
+        <color theme="1"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1481,9 +1090,19 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1532,9 +1151,131 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color auto="1"/>
         <name val="Aptos Narrow"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -1557,28 +1298,257 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color theme="1"/>
+        <color auto="1"/>
         <name val="Aptos Narrow"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1617,7 +1587,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color theme="1"/>
+        <color auto="1"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1626,19 +1596,9 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1677,7 +1637,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color theme="1"/>
+        <color auto="1"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1686,19 +1646,9 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1737,7 +1687,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color theme="1"/>
+        <color auto="1"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1746,19 +1696,9 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1797,27 +1737,18 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color theme="1"/>
+        <color auto="1"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1842,40 +1773,6 @@
           <bgColor theme="5" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1960,66 +1857,66 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{168AF483-6833-C345-BA9D-0EF06231DA67}" name="jtrn" displayName="jtrn" ref="A1:V41" totalsRowCount="1" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="A1:V40" xr:uid="{168AF483-6833-C345-BA9D-0EF06231DA67}"/>
   <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{53007CBC-089F-9844-888D-4AFD025D21A4}" name="Movement" totalsRowLabel="Subtotal" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{E7670F3E-FFC8-B44C-B726-CCCD0DDE580C}" name="Account Secondary" totalsRowLabel="Jeanre Transactional" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{BC34C8F0-D5A8-A942-ACF9-3833C647F3AA}" name="2024-05-01" totalsRowFunction="custom" dataDxfId="41" totalsRowDxfId="40">
+    <tableColumn id="1" xr3:uid="{53007CBC-089F-9844-888D-4AFD025D21A4}" name="Movement" totalsRowLabel="Subtotal" dataDxfId="45" totalsRowDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{E7670F3E-FFC8-B44C-B726-CCCD0DDE580C}" name="Account Secondary" totalsRowLabel="Jeanre Transactional" dataDxfId="44" totalsRowDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{BC34C8F0-D5A8-A942-ACF9-3833C647F3AA}" name="2024-05-01" totalsRowFunction="custom" dataDxfId="43" totalsRowDxfId="19">
       <totalsRowFormula>SUMIF('Jeanre Transactional'!$A$2:$A$41,"Credit", 'Jeanre Transactional'!$C$2:$C$41)-SUMIF('Jeanre Transactional'!$A$2:$A$41,"Debit", 'Jeanre Transactional'!$C$2:$C$41)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{12E99681-3EF3-154C-81F1-3C68ABFA379F}" name="2024-06-01" totalsRowFunction="custom" dataDxfId="39" totalsRowDxfId="38">
+    <tableColumn id="4" xr3:uid="{12E99681-3EF3-154C-81F1-3C68ABFA379F}" name="2024-06-01" totalsRowFunction="custom" dataDxfId="42" totalsRowDxfId="18">
       <totalsRowFormula>SUMIF('Jeanre Transactional'!$A$2:$A$41,"Credit", 'Jeanre Transactional'!$D$2:$D$41)-SUMIF('Jeanre Transactional'!$A$2:$A$41,"Debit", 'Jeanre Transactional'!$D$2:$D$41)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F853A505-CD2D-424A-AB56-7C307ACC3B35}" name="2024-07-01" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="36">
+    <tableColumn id="5" xr3:uid="{F853A505-CD2D-424A-AB56-7C307ACC3B35}" name="2024-07-01" totalsRowFunction="custom" dataDxfId="41" totalsRowDxfId="17">
       <totalsRowFormula>SUMIF('Jeanre Transactional'!$A$2:$A$41,"Credit", 'Jeanre Transactional'!$E$2:$E$41)-SUMIF('Jeanre Transactional'!$A$2:$A$41,"Debit", 'Jeanre Transactional'!$E$2:$E$41)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{7A5E017B-4309-9E43-8312-61D7567F2717}" name="2024-08-01" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="34">
+    <tableColumn id="6" xr3:uid="{7A5E017B-4309-9E43-8312-61D7567F2717}" name="2024-08-01" totalsRowFunction="custom" dataDxfId="40" totalsRowDxfId="16">
       <totalsRowFormula>SUMIF('Jeanre Transactional'!$A$2:$A$41,"Credit", 'Jeanre Transactional'!$F$2:$F$41)-SUMIF('Jeanre Transactional'!$A$2:$A$41,"Debit", 'Jeanre Transactional'!$F$2:$F$41)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{35A69827-17E6-D747-80AA-A3903629E38D}" name="2024-09-01" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="32">
+    <tableColumn id="7" xr3:uid="{35A69827-17E6-D747-80AA-A3903629E38D}" name="2024-09-01" totalsRowFunction="custom" dataDxfId="39" totalsRowDxfId="15">
       <totalsRowFormula>SUMIF('Jeanre Transactional'!$A$2:$A$41,"Credit", 'Jeanre Transactional'!$G$2:$G$41)-SUMIF('Jeanre Transactional'!$A$2:$A$41,"Debit", 'Jeanre Transactional'!$G$2:$G$41)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{07201ECD-0600-9049-8CF3-536066F50B85}" name="2024-10-01" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="30">
+    <tableColumn id="8" xr3:uid="{07201ECD-0600-9049-8CF3-536066F50B85}" name="2024-10-01" totalsRowFunction="custom" dataDxfId="38" totalsRowDxfId="14">
       <totalsRowFormula>SUMIF('Jeanre Transactional'!$A$2:$A$41,"Credit", 'Jeanre Transactional'!$H$2:$H$41)-SUMIF('Jeanre Transactional'!$A$2:$A$41,"Debit", 'Jeanre Transactional'!$H$2:$H$41)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{95C89772-EB84-6148-A713-02DB6582171E}" name="2024-11-01" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="28">
+    <tableColumn id="9" xr3:uid="{95C89772-EB84-6148-A713-02DB6582171E}" name="2024-11-01" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="13">
       <totalsRowFormula>SUMIF('Jeanre Transactional'!$A$2:$A$41,"Credit", 'Jeanre Transactional'!$I$2:$I$41)-SUMIF('Jeanre Transactional'!$A$2:$A$41,"Debit", 'Jeanre Transactional'!$I$2:$I$41)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{78C2C3D1-00C3-B447-A15B-F22E336A2B58}" name="2024-12-01" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="26">
+    <tableColumn id="10" xr3:uid="{78C2C3D1-00C3-B447-A15B-F22E336A2B58}" name="2024-12-01" totalsRowFunction="custom" dataDxfId="36" totalsRowDxfId="12">
       <totalsRowFormula>SUMIF('Jeanre Transactional'!$A$2:$A$41,"Credit", 'Jeanre Transactional'!$J$2:$J$41)-SUMIF('Jeanre Transactional'!$A$2:$A$41,"Debit", 'Jeanre Transactional'!$J$2:$J$41)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{A6168F27-4891-0749-92DD-57A77D1DACAA}" name="2025-01-01" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="24">
+    <tableColumn id="11" xr3:uid="{A6168F27-4891-0749-92DD-57A77D1DACAA}" name="2025-01-01" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="11">
       <totalsRowFormula>SUMIF(jtrn[Movement], "Credit", jtrn[2025-01-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-01-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{58BC0315-6C75-9548-B003-5335630C1315}" name="2025-02-01" totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="22">
+    <tableColumn id="12" xr3:uid="{58BC0315-6C75-9548-B003-5335630C1315}" name="2025-02-01" totalsRowFunction="custom" dataDxfId="34" totalsRowDxfId="10">
       <totalsRowFormula>SUMIF(jtrn[Movement], "Credit", jtrn[2025-02-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-02-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{896888D1-CC44-3042-B2FE-75BF30E0F183}" name="2025-03-01" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="20">
+    <tableColumn id="13" xr3:uid="{896888D1-CC44-3042-B2FE-75BF30E0F183}" name="2025-03-01" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="9">
       <totalsRowFormula>SUMIF(jtrn[Movement], "Credit", jtrn[2025-03-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-03-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{1670E3CE-2F37-E048-813C-B7C337151740}" name="2025-04-01" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="18">
+    <tableColumn id="14" xr3:uid="{1670E3CE-2F37-E048-813C-B7C337151740}" name="2025-04-01" totalsRowFunction="custom" dataDxfId="32" totalsRowDxfId="8">
       <totalsRowFormula>SUMIF(jtrn[Movement], "Credit", jtrn[2025-04-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-04-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{6572C763-49E9-AA4F-9718-2BC9B7E57762}" name="2025-05-01" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="16">
+    <tableColumn id="15" xr3:uid="{6572C763-49E9-AA4F-9718-2BC9B7E57762}" name="2025-05-01" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="7">
       <totalsRowFormula>SUMIF(jtrn[Movement], "Credit", jtrn[2025-05-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-05-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{99AC582F-E016-EB4C-A534-6BAC5A7AD88A}" name="2025-06-01" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="14">
+    <tableColumn id="16" xr3:uid="{99AC582F-E016-EB4C-A534-6BAC5A7AD88A}" name="2025-06-01" totalsRowFunction="custom" dataDxfId="30" totalsRowDxfId="6">
       <totalsRowFormula>SUMIF(jtrn[Movement], "Credit", jtrn[2025-06-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-06-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{2AFE4E94-A26F-1648-B078-CC1ACB60F61E}" name="2025-07-01" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="12">
+    <tableColumn id="17" xr3:uid="{2AFE4E94-A26F-1648-B078-CC1ACB60F61E}" name="2025-07-01" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="5">
       <totalsRowFormula>SUMIF(jtrn[Movement], "Credit", jtrn[2025-07-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-07-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{9169B43F-AE90-B84E-BB9B-3E2730E4B499}" name="2025-08-01" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
+    <tableColumn id="18" xr3:uid="{9169B43F-AE90-B84E-BB9B-3E2730E4B499}" name="2025-08-01" totalsRowFunction="custom" dataDxfId="28" totalsRowDxfId="4">
       <totalsRowFormula>SUMIF(jtrn[Movement], "Credit", jtrn[2025-08-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-08-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{16A4B7C1-DCCD-BC42-80A2-5A9B0AFE62B7}" name="2025-09-01" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="8">
+    <tableColumn id="19" xr3:uid="{16A4B7C1-DCCD-BC42-80A2-5A9B0AFE62B7}" name="2025-09-01" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="3">
       <totalsRowFormula>SUMIF(jtrn[Movement], "Credit", jtrn[2025-09-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-09-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{DA0D9353-5004-BC49-A034-377720B302FE}" name="2025-10-01" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="6">
+    <tableColumn id="20" xr3:uid="{DA0D9353-5004-BC49-A034-377720B302FE}" name="2025-10-01" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="2">
       <totalsRowFormula>SUMIF(jtrn[Movement], "Credit", jtrn[2025-10-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-10-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{2CAF52BB-84EF-4B4E-9560-96A6E500A093}" name="2025-11-01" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4">
+    <tableColumn id="21" xr3:uid="{2CAF52BB-84EF-4B4E-9560-96A6E500A093}" name="2025-11-01" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="1">
       <totalsRowFormula>SUMIF(jtrn[Movement], "Credit", jtrn[2025-11-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-11-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{2627D4F2-2727-3545-907E-0FB0C0AA352F}" name="2025-12-01" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="2">
+    <tableColumn id="22" xr3:uid="{2627D4F2-2727-3545-907E-0FB0C0AA352F}" name="2025-12-01" totalsRowFunction="custom" dataDxfId="24" totalsRowDxfId="0">
       <totalsRowFormula>SUMIF(jtrn[Movement], "Credit", jtrn[2025-12-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-12-01])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -2345,21 +2242,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392F97BE-146F-BF41-B2C2-34275CA1ADBB}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AC79"/>
+  <dimension ref="A1:AD70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="109" workbookViewId="0">
+      <selection activeCell="S75" sqref="S75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="5" width="15.1640625" style="1" customWidth="1"/>
-    <col min="6" max="11" width="15.1640625" customWidth="1"/>
-    <col min="12" max="12" width="19" customWidth="1"/>
-    <col min="13" max="22" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20" hidden="1" customWidth="1"/>
+    <col min="4" max="5" width="15.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="11" width="15.1640625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="19" hidden="1" customWidth="1"/>
+    <col min="13" max="16" width="19.33203125" hidden="1" customWidth="1"/>
+    <col min="17" max="22" width="19.33203125" customWidth="1"/>
     <col min="28" max="28" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2548,8 +2446,8 @@
       <c r="P3" s="7">
         <v>1349</v>
       </c>
-      <c r="Q3" s="8">
-        <v>1419</v>
+      <c r="Q3" s="7">
+        <v>1349</v>
       </c>
       <c r="R3" s="8">
         <v>1169</v>
@@ -2622,7 +2520,9 @@
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
+      <c r="Q5" s="7">
+        <v>300</v>
+      </c>
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
       <c r="T5" s="8"/>
@@ -2695,23 +2595,23 @@
       </c>
       <c r="R7" s="8">
         <f>jtrn[[#Totals],[2025-07-01]]</f>
-        <v>135</v>
+        <v>1367</v>
       </c>
       <c r="S7" s="8">
         <f>jtrn[[#Totals],[2025-08-01]]</f>
-        <v>1090</v>
+        <v>1822</v>
       </c>
       <c r="T7" s="8">
         <f>jtrn[[#Totals],[2025-09-01]]</f>
-        <v>6145</v>
+        <v>6877</v>
       </c>
       <c r="U7" s="8">
         <f>jtrn[[#Totals],[2025-10-01]]</f>
-        <v>6900</v>
+        <v>7632</v>
       </c>
       <c r="V7" s="8">
         <f>jtrn[[#Totals],[2025-11-01]]</f>
-        <v>5655</v>
+        <v>6387</v>
       </c>
     </row>
     <row r="8" spans="1:22" s="2" customFormat="1" ht="22" x14ac:dyDescent="0.3">
@@ -2795,7 +2695,7 @@
       <c r="P9" s="7">
         <v>8000</v>
       </c>
-      <c r="Q9" s="8">
+      <c r="Q9" s="7">
         <v>8000</v>
       </c>
       <c r="R9" s="8">
@@ -2931,7 +2831,7 @@
       <c r="P11" s="32">
         <v>7795</v>
       </c>
-      <c r="Q11" s="12">
+      <c r="Q11" s="32">
         <v>7795</v>
       </c>
       <c r="R11" s="12">
@@ -3064,10 +2964,10 @@
       <c r="O13" s="33">
         <v>6305</v>
       </c>
-      <c r="P13" s="48">
+      <c r="P13" s="40">
         <v>6305</v>
       </c>
-      <c r="Q13" s="10">
+      <c r="Q13" s="33">
         <v>6305</v>
       </c>
       <c r="R13" s="10">
@@ -3135,7 +3035,7 @@
       <c r="P14" s="32">
         <v>170</v>
       </c>
-      <c r="Q14" s="12">
+      <c r="Q14" s="32">
         <v>170</v>
       </c>
       <c r="R14" s="12">
@@ -3203,7 +3103,7 @@
       <c r="P15" s="33">
         <v>117</v>
       </c>
-      <c r="Q15" s="10">
+      <c r="Q15" s="33">
         <v>117</v>
       </c>
       <c r="R15" s="10">
@@ -3262,16 +3162,16 @@
       <c r="M16" s="35">
         <v>690</v>
       </c>
-      <c r="N16" s="46">
+      <c r="N16" s="38">
         <v>690</v>
       </c>
       <c r="O16" s="32">
         <v>855</v>
       </c>
-      <c r="P16" s="49">
+      <c r="P16" s="41">
         <v>690</v>
       </c>
-      <c r="Q16" s="12">
+      <c r="Q16" s="32">
         <v>690</v>
       </c>
       <c r="R16" s="12">
@@ -3330,7 +3230,7 @@
       <c r="M17" s="36">
         <v>610</v>
       </c>
-      <c r="N17" s="47">
+      <c r="N17" s="39">
         <v>610</v>
       </c>
       <c r="O17" s="33">
@@ -3339,7 +3239,7 @@
       <c r="P17" s="33">
         <v>610</v>
       </c>
-      <c r="Q17" s="10">
+      <c r="Q17" s="33">
         <v>610</v>
       </c>
       <c r="R17" s="10">
@@ -3407,7 +3307,7 @@
       <c r="P18" s="32">
         <v>450</v>
       </c>
-      <c r="Q18" s="12">
+      <c r="Q18" s="32">
         <v>450</v>
       </c>
       <c r="R18" s="12">
@@ -3475,8 +3375,8 @@
       <c r="P19" s="33">
         <v>4100</v>
       </c>
-      <c r="Q19" s="10">
-        <v>3200</v>
+      <c r="Q19" s="40">
+        <v>0</v>
       </c>
       <c r="R19" s="10">
         <v>3200</v>
@@ -3612,7 +3512,7 @@
         <v>1000</v>
       </c>
       <c r="Q21" s="33">
-        <v>400</v>
+        <v>550</v>
       </c>
       <c r="R21" s="10">
         <v>400</v>
@@ -3679,8 +3579,8 @@
       <c r="P22" s="12">
         <v>3700</v>
       </c>
-      <c r="Q22" s="12">
-        <v>3500</v>
+      <c r="Q22" s="41">
+        <v>5928</v>
       </c>
       <c r="R22" s="12">
         <v>3700</v>
@@ -3999,8 +3899,8 @@
       <c r="N28" s="12"/>
       <c r="O28" s="12"/>
       <c r="P28" s="12"/>
-      <c r="Q28" s="12">
-        <v>630</v>
+      <c r="Q28" s="32">
+        <v>750</v>
       </c>
       <c r="R28" s="12"/>
       <c r="S28" s="12"/>
@@ -4067,7 +3967,7 @@
       <c r="N30" s="12"/>
       <c r="O30" s="12"/>
       <c r="P30" s="12"/>
-      <c r="Q30" s="12">
+      <c r="Q30" s="32">
         <v>1090</v>
       </c>
       <c r="R30" s="12"/>
@@ -4156,7 +4056,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="33" spans="1:22" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:30" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
         <v>35</v>
       </c>
@@ -4182,13 +4082,15 @@
       <c r="O33" s="12"/>
       <c r="P33" s="12"/>
       <c r="Q33" s="12"/>
-      <c r="R33" s="12"/>
+      <c r="R33" s="12">
+        <v>500</v>
+      </c>
       <c r="S33" s="12"/>
       <c r="T33" s="12"/>
       <c r="U33" s="12"/>
       <c r="V33" s="12"/>
     </row>
-    <row r="34" spans="1:22" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:30" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
         <v>35</v>
       </c>
@@ -4234,7 +4136,7 @@
       <c r="U34" s="12"/>
       <c r="V34" s="12"/>
     </row>
-    <row r="35" spans="1:22" s="11" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:30" s="11" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
         <v>35</v>
       </c>
@@ -4280,7 +4182,7 @@
       <c r="U35" s="12"/>
       <c r="V35" s="12"/>
     </row>
-    <row r="36" spans="1:22" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:30" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
         <v>35</v>
       </c>
@@ -4308,12 +4210,12 @@
       <c r="U36" s="12"/>
       <c r="V36" s="12"/>
     </row>
-    <row r="37" spans="1:22" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:30" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="C37" s="25"/>
       <c r="D37" s="25"/>
@@ -4354,7 +4256,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:22" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:30" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
         <v>35</v>
       </c>
@@ -4388,12 +4290,12 @@
       <c r="U38" s="12"/>
       <c r="V38" s="12"/>
     </row>
-    <row r="39" spans="1:22" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:30" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>104</v>
+        <v>66</v>
       </c>
       <c r="C39" s="25"/>
       <c r="D39" s="25"/>
@@ -4409,16 +4311,14 @@
       <c r="N39" s="12"/>
       <c r="O39" s="12"/>
       <c r="P39" s="12"/>
-      <c r="Q39" s="12">
-        <v>500</v>
-      </c>
+      <c r="Q39" s="12"/>
       <c r="R39" s="12"/>
       <c r="S39" s="12"/>
       <c r="T39" s="12"/>
       <c r="U39" s="12"/>
       <c r="V39" s="12"/>
     </row>
-    <row r="40" spans="1:22" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:30" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
         <v>35</v>
       </c>
@@ -4478,7 +4378,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="41" spans="1:22" ht="22" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:30" ht="22" x14ac:dyDescent="0.3">
       <c r="A41" s="30" t="s">
         <v>48</v>
       </c>
@@ -4543,32 +4443,32 @@
       </c>
       <c r="Q41" s="5">
         <f>SUMIF(jtrn[Movement], "Credit", jtrn[2025-07-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-07-01])</f>
-        <v>135</v>
+        <v>1367</v>
       </c>
       <c r="R41" s="5">
         <f>SUMIF(jtrn[Movement], "Credit", jtrn[2025-08-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-08-01])</f>
-        <v>1090</v>
+        <v>1822</v>
       </c>
       <c r="S41" s="5">
         <f>SUMIF(jtrn[Movement], "Credit", jtrn[2025-09-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-09-01])</f>
-        <v>6145</v>
+        <v>6877</v>
       </c>
       <c r="T41" s="5">
         <f>SUMIF(jtrn[Movement], "Credit", jtrn[2025-10-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-10-01])</f>
-        <v>6900</v>
+        <v>7632</v>
       </c>
       <c r="U41" s="5">
         <f>SUMIF(jtrn[Movement], "Credit", jtrn[2025-11-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-11-01])</f>
-        <v>5655</v>
+        <v>6387</v>
       </c>
       <c r="V41" s="5">
         <f>SUMIF(jtrn[Movement], "Credit", jtrn[2025-12-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-12-01])</f>
-        <v>6410</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22" ht="22" x14ac:dyDescent="0.3">
+        <v>7142</v>
+      </c>
+    </row>
+    <row r="42" spans="1:30" ht="22" x14ac:dyDescent="0.3">
       <c r="A42" s="30" t="s">
-        <v>101</v>
+        <v>63</v>
       </c>
       <c r="B42" s="30" t="s">
         <v>0</v>
@@ -4631,11 +4531,11 @@
       </c>
       <c r="Q42" s="5">
         <f>SUMIF(jtrn[Movement], "Credit", jtrn[2025-07-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-07-01])- SUMIF(jtrn[Account Secondary], "Retained Balance", jtrn[2025-07-01])</f>
-        <v>-765</v>
+        <v>467</v>
       </c>
       <c r="R42" s="5">
         <f>SUMIF(jtrn[Movement], "Credit", jtrn[2025-08-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-08-01])- SUMIF(jtrn[Account Secondary], "Retained Balance", jtrn[2025-08-01])</f>
-        <v>955</v>
+        <v>455</v>
       </c>
       <c r="S42" s="5">
         <f>SUMIF(jtrn[Movement], "Credit", jtrn[2025-09-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-09-01])- SUMIF(jtrn[Account Secondary], "Retained Balance", jtrn[2025-09-01])</f>
@@ -4654,418 +4554,222 @@
         <v>755</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
       <c r="O46" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="51" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B51" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q46" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="R46" s="44">
+        <v>250</v>
+      </c>
+      <c r="S46" t="s">
+        <v>67</v>
+      </c>
+      <c r="T46">
+        <v>10545.22</v>
+      </c>
+      <c r="V46" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="W46" s="42">
+        <v>1697</v>
+      </c>
+      <c r="Z46" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA46" s="42">
+        <v>300</v>
+      </c>
+      <c r="AB46" s="42"/>
+      <c r="AC46" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="C51" s="39"/>
-      <c r="D51" s="38"/>
-      <c r="E51" s="38"/>
-      <c r="F51" s="39"/>
-      <c r="G51" s="39"/>
-      <c r="H51" s="39"/>
-      <c r="I51" s="39"/>
-      <c r="J51" s="39"/>
-      <c r="K51" s="39"/>
-      <c r="L51" s="39"/>
-      <c r="M51" s="38">
-        <v>3700</v>
-      </c>
-    </row>
-    <row r="52" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B52" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="C52" s="39"/>
-      <c r="D52" s="38"/>
-      <c r="E52" s="38"/>
-      <c r="F52" s="39"/>
-      <c r="G52" s="39"/>
-      <c r="H52" s="39"/>
-      <c r="I52" s="39"/>
-      <c r="J52" s="39"/>
-      <c r="K52" s="39"/>
-      <c r="L52" s="39"/>
-      <c r="M52" s="39">
-        <v>1600</v>
-      </c>
-      <c r="P52" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q52">
-        <v>1600</v>
-      </c>
-      <c r="R52" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="53" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B53" s="39" t="s">
+      <c r="AD46" s="42">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="S47" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="T47" s="45">
+        <v>6305</v>
+      </c>
+      <c r="V47" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="W47" s="42">
+        <v>70</v>
+      </c>
+      <c r="Z47" s="42"/>
+      <c r="AA47" s="42"/>
+      <c r="AB47" s="42"/>
+      <c r="AC47" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD47" s="42">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="S48" t="s">
+        <v>78</v>
+      </c>
+      <c r="T48">
+        <v>3445</v>
+      </c>
+      <c r="U48" t="s">
+        <v>83</v>
+      </c>
+      <c r="V48" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="C53" s="39"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="38"/>
-      <c r="F53" s="39"/>
-      <c r="G53" s="39"/>
-      <c r="H53" s="39"/>
-      <c r="I53" s="39"/>
-      <c r="J53" s="39"/>
-      <c r="K53" s="39"/>
-      <c r="L53" s="39"/>
-      <c r="M53" s="39">
-        <v>1000</v>
-      </c>
-      <c r="P53" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q53">
-        <v>3510</v>
-      </c>
-      <c r="R53" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="54" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B54" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="C54" s="39"/>
-      <c r="D54" s="38"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="39"/>
-      <c r="G54" s="39"/>
-      <c r="H54" s="39"/>
-      <c r="I54" s="39"/>
-      <c r="J54" s="39"/>
-      <c r="K54" s="39"/>
-      <c r="L54" s="39"/>
-      <c r="M54" s="39"/>
-      <c r="P54" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q54">
-        <v>90</v>
-      </c>
-      <c r="R54" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="55" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="C55" s="42"/>
-      <c r="D55" s="43"/>
-      <c r="E55" s="43"/>
-      <c r="F55" s="42"/>
-      <c r="G55" s="42"/>
-      <c r="H55" s="42"/>
-      <c r="I55" s="42"/>
-      <c r="J55" s="42"/>
-      <c r="K55" s="42"/>
-      <c r="L55" s="42"/>
-      <c r="M55" s="42">
-        <v>800</v>
-      </c>
-      <c r="P55" t="s">
+      <c r="W48" s="42">
+        <v>2234</v>
+      </c>
+    </row>
+    <row r="49" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S49" t="s">
+        <v>79</v>
+      </c>
+      <c r="T49">
+        <v>2508</v>
+      </c>
+      <c r="U49" t="s">
+        <v>83</v>
+      </c>
+      <c r="V49" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="Q55">
-        <v>60</v>
-      </c>
-      <c r="R55" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="56" spans="2:19" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="40" t="s">
-        <v>65</v>
-      </c>
-      <c r="C56" s="40"/>
-      <c r="D56" s="41"/>
-      <c r="E56" s="41"/>
-      <c r="F56" s="40"/>
-      <c r="G56" s="40"/>
-      <c r="H56" s="40"/>
-      <c r="I56" s="40"/>
-      <c r="J56" s="40"/>
-      <c r="K56" s="40"/>
-      <c r="L56" s="40"/>
-      <c r="M56" s="40">
-        <f>M51-SUM(M52:M55)</f>
-        <v>300</v>
-      </c>
-      <c r="P56" t="s">
+      <c r="W49" s="42">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="T50" s="43">
+        <f>SUM(T46:T49)</f>
+        <v>22803.22</v>
+      </c>
+      <c r="V50" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="Q56">
-        <v>170</v>
-      </c>
-      <c r="R56" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="57" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="P57" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q57">
-        <v>50</v>
-      </c>
-      <c r="R57" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="58" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="P58" t="s">
+      <c r="W50" s="42">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="V51" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="Q58">
+      <c r="W51" s="42">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="52" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="V52" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="W52" s="42">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="53" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S53" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="T53" s="42">
+        <v>1090</v>
+      </c>
+      <c r="V53" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="W53" s="42">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="54" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="V54" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="W54" s="42">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="55" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S55" t="s">
+        <v>82</v>
+      </c>
+      <c r="T55">
+        <v>700</v>
+      </c>
+      <c r="V55" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="W55" s="42">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="V56" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="W56" s="42">
         <v>290</v>
       </c>
-      <c r="R58" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="59" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="I59">
-        <f>SUMIF('Jeanre Transactional'!$A$2:$A$41,"Credit", 'Jeanre Transactional'!$J$2:$J$41)-SUMIF('Jeanre Transactional'!$A$2:$A$41,"Debit", 'Jeanre Transactional'!$J$2:$J$41)</f>
-        <v>-174</v>
-      </c>
-      <c r="P59" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q59" s="45">
-        <v>500</v>
-      </c>
-      <c r="R59" s="45" t="s">
-        <v>66</v>
-      </c>
-      <c r="S59" s="45" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="60" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="P60" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q60">
-        <v>304</v>
-      </c>
-      <c r="R60" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="61" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="P61" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q61">
-        <v>12</v>
-      </c>
-      <c r="R61" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="62" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="P62" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q62">
-        <v>110</v>
-      </c>
-      <c r="R62" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="63" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="P63" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q63">
-        <v>320</v>
-      </c>
-      <c r="R63" t="s">
-        <v>66</v>
-      </c>
-      <c r="S63" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="64" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="P64" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q64">
-        <v>500</v>
-      </c>
-      <c r="R64" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="65" spans="16:29" x14ac:dyDescent="0.2">
-      <c r="P65" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q65">
-        <v>41</v>
-      </c>
-      <c r="R65" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="66" spans="16:29" x14ac:dyDescent="0.2">
-      <c r="P66" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q66">
-        <v>154</v>
-      </c>
-      <c r="R66" t="s">
-        <v>66</v>
-      </c>
+    </row>
+    <row r="57" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="V57" s="42"/>
+      <c r="W57" s="42">
+        <f>SUM(W46:W56)</f>
+        <v>5928</v>
+      </c>
+    </row>
+    <row r="66" spans="19:22" x14ac:dyDescent="0.2">
       <c r="S66" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="67" spans="16:29" x14ac:dyDescent="0.2">
-      <c r="P67" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q67">
-        <v>451</v>
-      </c>
-      <c r="R67" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="68" spans="16:29" x14ac:dyDescent="0.2">
-      <c r="P68" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q68">
-        <v>1382</v>
-      </c>
-      <c r="R68" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="69" spans="16:29" x14ac:dyDescent="0.2">
-      <c r="P69" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q69">
-        <v>40</v>
-      </c>
-      <c r="R69" t="s">
-        <v>81</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="T66">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="68" spans="19:22" x14ac:dyDescent="0.2">
+      <c r="S68" t="s">
+        <v>61</v>
+      </c>
+      <c r="T68">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="69" spans="19:22" x14ac:dyDescent="0.2">
       <c r="S69" t="s">
-        <v>88</v>
-      </c>
-      <c r="T69" s="44" t="s">
-        <v>90</v>
-      </c>
-      <c r="X69" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y69">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="70" spans="16:29" x14ac:dyDescent="0.2">
-      <c r="X70" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y70" s="44">
-        <v>2627</v>
-      </c>
-      <c r="Z70" s="44" t="s">
-        <v>98</v>
-      </c>
-      <c r="AA70" s="44"/>
-    </row>
-    <row r="71" spans="16:29" x14ac:dyDescent="0.2">
-      <c r="Y71">
-        <f>SUM(Y69:Y70)</f>
-        <v>3273</v>
-      </c>
-    </row>
-    <row r="74" spans="16:29" x14ac:dyDescent="0.2">
-      <c r="P74" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q74">
-        <f>SUM(Q52:Q69)</f>
-        <v>9584</v>
-      </c>
-      <c r="S74" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="75" spans="16:29" x14ac:dyDescent="0.2">
-      <c r="S75" t="s">
+      <c r="T69">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="70" spans="19:22" x14ac:dyDescent="0.2">
+      <c r="T70" s="45">
+        <f>SUM(T66:T69)</f>
+        <v>2811</v>
+      </c>
+      <c r="U70" s="45">
+        <f>T47-T70</f>
+        <v>3494</v>
+      </c>
+      <c r="V70" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="76" spans="16:29" x14ac:dyDescent="0.2">
-      <c r="S76" t="s">
-        <v>86</v>
-      </c>
-      <c r="X76" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y76" s="44">
-        <v>3516</v>
-      </c>
-      <c r="Z76" s="44" t="s">
-        <v>99</v>
-      </c>
-      <c r="AA76" s="44">
-        <v>2373</v>
-      </c>
-      <c r="AB76" s="44" t="s">
-        <v>100</v>
-      </c>
-      <c r="AC76" s="44">
-        <v>1143</v>
-      </c>
-    </row>
-    <row r="77" spans="16:29" x14ac:dyDescent="0.2">
-      <c r="S77" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="X77" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y77">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="79" spans="16:29" x14ac:dyDescent="0.2">
-      <c r="U79" t="s">
-        <v>96</v>
-      </c>
-      <c r="X79" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y79" s="1">
-        <v>1143</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="M41:V42">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fix simulation interest compounding logic and add financial calculator section
Changed files:
- start.html: Added Financial Calculator section to the UI for compound interest and annuity calculations
- styles/simulation.css: Added styles for the calculator section and result display
- function/simulation.js: Fixed simulation logic to use correct compounding period and per-period rate, added calculator logic for all major formulas, and improved interest handling.
</commit_message>
<xml_diff>
--- a/original-excel-sources/budget_jeanre.xlsx
+++ b/original-excel-sources/budget_jeanre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jay/GIT-Repos-Personal/ftrack/original-excel-sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD40F6A-CE18-C74C-8B10-EAEA73A320F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3179B2-D56E-644A-91FA-4AED95935528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-68800" yWindow="-10980" windowWidth="68800" windowHeight="28300" xr2:uid="{F25DD163-696E-F842-A897-5E899A2812A7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{F25DD163-696E-F842-A897-5E899A2812A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Jeanre Transactional" sheetId="11" r:id="rId1"/>
@@ -608,25 +608,21 @@
   <dxfs count="48">
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
+        <color rgb="FF9C0006"/>
       </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -666,7 +662,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color theme="1"/>
+        <color auto="1"/>
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
@@ -674,7 +670,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
     </dxf>
@@ -714,7 +710,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color theme="1"/>
+        <color auto="1"/>
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
@@ -722,7 +718,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
     </dxf>
@@ -762,7 +758,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color theme="1"/>
+        <color auto="1"/>
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
@@ -770,7 +766,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
     </dxf>
@@ -810,7 +806,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color theme="1"/>
+        <color auto="1"/>
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
@@ -818,7 +814,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
     </dxf>
@@ -858,6 +854,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color theme="1"/>
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
@@ -882,6 +902,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color theme="1"/>
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
@@ -891,6 +935,270 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
     </dxf>
@@ -941,7 +1249,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color theme="1"/>
+        <color auto="1"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -950,19 +1258,9 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1011,7 +1309,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color theme="1"/>
+        <color auto="1"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1020,19 +1318,9 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1081,7 +1369,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color theme="1"/>
+        <color auto="1"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1090,19 +1378,9 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1151,6 +1429,31 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <color theme="1"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
@@ -1173,382 +1476,6 @@
           <color theme="1"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1587,7 +1514,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color auto="1"/>
+        <color theme="1"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1596,9 +1523,19 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1637,7 +1574,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color auto="1"/>
+        <color theme="1"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1646,9 +1583,19 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1687,7 +1634,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color auto="1"/>
+        <color theme="1"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1696,9 +1643,19 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1737,18 +1694,27 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color auto="1"/>
+        <color theme="1"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;R&quot;* #,##0.00_);_(&quot;R&quot;* \(#,##0.00\);_(&quot;R&quot;* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1773,6 +1739,40 @@
           <bgColor theme="5" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1857,66 +1857,66 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{168AF483-6833-C345-BA9D-0EF06231DA67}" name="jtrn" displayName="jtrn" ref="A1:V41" totalsRowCount="1" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="A1:V40" xr:uid="{168AF483-6833-C345-BA9D-0EF06231DA67}"/>
   <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{53007CBC-089F-9844-888D-4AFD025D21A4}" name="Movement" totalsRowLabel="Subtotal" dataDxfId="45" totalsRowDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{E7670F3E-FFC8-B44C-B726-CCCD0DDE580C}" name="Account Secondary" totalsRowLabel="Jeanre Transactional" dataDxfId="44" totalsRowDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{BC34C8F0-D5A8-A942-ACF9-3833C647F3AA}" name="2024-05-01" totalsRowFunction="custom" dataDxfId="43" totalsRowDxfId="19">
+    <tableColumn id="1" xr3:uid="{53007CBC-089F-9844-888D-4AFD025D21A4}" name="Movement" totalsRowLabel="Subtotal" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{E7670F3E-FFC8-B44C-B726-CCCD0DDE580C}" name="Account Secondary" totalsRowLabel="Jeanre Transactional" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{BC34C8F0-D5A8-A942-ACF9-3833C647F3AA}" name="2024-05-01" totalsRowFunction="custom" dataDxfId="41" totalsRowDxfId="40">
       <totalsRowFormula>SUMIF('Jeanre Transactional'!$A$2:$A$41,"Credit", 'Jeanre Transactional'!$C$2:$C$41)-SUMIF('Jeanre Transactional'!$A$2:$A$41,"Debit", 'Jeanre Transactional'!$C$2:$C$41)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{12E99681-3EF3-154C-81F1-3C68ABFA379F}" name="2024-06-01" totalsRowFunction="custom" dataDxfId="42" totalsRowDxfId="18">
+    <tableColumn id="4" xr3:uid="{12E99681-3EF3-154C-81F1-3C68ABFA379F}" name="2024-06-01" totalsRowFunction="custom" dataDxfId="39" totalsRowDxfId="38">
       <totalsRowFormula>SUMIF('Jeanre Transactional'!$A$2:$A$41,"Credit", 'Jeanre Transactional'!$D$2:$D$41)-SUMIF('Jeanre Transactional'!$A$2:$A$41,"Debit", 'Jeanre Transactional'!$D$2:$D$41)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F853A505-CD2D-424A-AB56-7C307ACC3B35}" name="2024-07-01" totalsRowFunction="custom" dataDxfId="41" totalsRowDxfId="17">
+    <tableColumn id="5" xr3:uid="{F853A505-CD2D-424A-AB56-7C307ACC3B35}" name="2024-07-01" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="36">
       <totalsRowFormula>SUMIF('Jeanre Transactional'!$A$2:$A$41,"Credit", 'Jeanre Transactional'!$E$2:$E$41)-SUMIF('Jeanre Transactional'!$A$2:$A$41,"Debit", 'Jeanre Transactional'!$E$2:$E$41)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{7A5E017B-4309-9E43-8312-61D7567F2717}" name="2024-08-01" totalsRowFunction="custom" dataDxfId="40" totalsRowDxfId="16">
+    <tableColumn id="6" xr3:uid="{7A5E017B-4309-9E43-8312-61D7567F2717}" name="2024-08-01" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="34">
       <totalsRowFormula>SUMIF('Jeanre Transactional'!$A$2:$A$41,"Credit", 'Jeanre Transactional'!$F$2:$F$41)-SUMIF('Jeanre Transactional'!$A$2:$A$41,"Debit", 'Jeanre Transactional'!$F$2:$F$41)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{35A69827-17E6-D747-80AA-A3903629E38D}" name="2024-09-01" totalsRowFunction="custom" dataDxfId="39" totalsRowDxfId="15">
+    <tableColumn id="7" xr3:uid="{35A69827-17E6-D747-80AA-A3903629E38D}" name="2024-09-01" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="32">
       <totalsRowFormula>SUMIF('Jeanre Transactional'!$A$2:$A$41,"Credit", 'Jeanre Transactional'!$G$2:$G$41)-SUMIF('Jeanre Transactional'!$A$2:$A$41,"Debit", 'Jeanre Transactional'!$G$2:$G$41)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{07201ECD-0600-9049-8CF3-536066F50B85}" name="2024-10-01" totalsRowFunction="custom" dataDxfId="38" totalsRowDxfId="14">
+    <tableColumn id="8" xr3:uid="{07201ECD-0600-9049-8CF3-536066F50B85}" name="2024-10-01" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="30">
       <totalsRowFormula>SUMIF('Jeanre Transactional'!$A$2:$A$41,"Credit", 'Jeanre Transactional'!$H$2:$H$41)-SUMIF('Jeanre Transactional'!$A$2:$A$41,"Debit", 'Jeanre Transactional'!$H$2:$H$41)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{95C89772-EB84-6148-A713-02DB6582171E}" name="2024-11-01" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="13">
+    <tableColumn id="9" xr3:uid="{95C89772-EB84-6148-A713-02DB6582171E}" name="2024-11-01" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="28">
       <totalsRowFormula>SUMIF('Jeanre Transactional'!$A$2:$A$41,"Credit", 'Jeanre Transactional'!$I$2:$I$41)-SUMIF('Jeanre Transactional'!$A$2:$A$41,"Debit", 'Jeanre Transactional'!$I$2:$I$41)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{78C2C3D1-00C3-B447-A15B-F22E336A2B58}" name="2024-12-01" totalsRowFunction="custom" dataDxfId="36" totalsRowDxfId="12">
+    <tableColumn id="10" xr3:uid="{78C2C3D1-00C3-B447-A15B-F22E336A2B58}" name="2024-12-01" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="26">
       <totalsRowFormula>SUMIF('Jeanre Transactional'!$A$2:$A$41,"Credit", 'Jeanre Transactional'!$J$2:$J$41)-SUMIF('Jeanre Transactional'!$A$2:$A$41,"Debit", 'Jeanre Transactional'!$J$2:$J$41)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{A6168F27-4891-0749-92DD-57A77D1DACAA}" name="2025-01-01" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="11">
+    <tableColumn id="11" xr3:uid="{A6168F27-4891-0749-92DD-57A77D1DACAA}" name="2025-01-01" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="24">
       <totalsRowFormula>SUMIF(jtrn[Movement], "Credit", jtrn[2025-01-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-01-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{58BC0315-6C75-9548-B003-5335630C1315}" name="2025-02-01" totalsRowFunction="custom" dataDxfId="34" totalsRowDxfId="10">
+    <tableColumn id="12" xr3:uid="{58BC0315-6C75-9548-B003-5335630C1315}" name="2025-02-01" totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="22">
       <totalsRowFormula>SUMIF(jtrn[Movement], "Credit", jtrn[2025-02-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-02-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{896888D1-CC44-3042-B2FE-75BF30E0F183}" name="2025-03-01" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="9">
+    <tableColumn id="13" xr3:uid="{896888D1-CC44-3042-B2FE-75BF30E0F183}" name="2025-03-01" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="20">
       <totalsRowFormula>SUMIF(jtrn[Movement], "Credit", jtrn[2025-03-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-03-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{1670E3CE-2F37-E048-813C-B7C337151740}" name="2025-04-01" totalsRowFunction="custom" dataDxfId="32" totalsRowDxfId="8">
+    <tableColumn id="14" xr3:uid="{1670E3CE-2F37-E048-813C-B7C337151740}" name="2025-04-01" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="18">
       <totalsRowFormula>SUMIF(jtrn[Movement], "Credit", jtrn[2025-04-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-04-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{6572C763-49E9-AA4F-9718-2BC9B7E57762}" name="2025-05-01" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="7">
+    <tableColumn id="15" xr3:uid="{6572C763-49E9-AA4F-9718-2BC9B7E57762}" name="2025-05-01" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="16">
       <totalsRowFormula>SUMIF(jtrn[Movement], "Credit", jtrn[2025-05-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-05-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{99AC582F-E016-EB4C-A534-6BAC5A7AD88A}" name="2025-06-01" totalsRowFunction="custom" dataDxfId="30" totalsRowDxfId="6">
+    <tableColumn id="16" xr3:uid="{99AC582F-E016-EB4C-A534-6BAC5A7AD88A}" name="2025-06-01" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="14">
       <totalsRowFormula>SUMIF(jtrn[Movement], "Credit", jtrn[2025-06-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-06-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{2AFE4E94-A26F-1648-B078-CC1ACB60F61E}" name="2025-07-01" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="5">
+    <tableColumn id="17" xr3:uid="{2AFE4E94-A26F-1648-B078-CC1ACB60F61E}" name="2025-07-01" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="12">
       <totalsRowFormula>SUMIF(jtrn[Movement], "Credit", jtrn[2025-07-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-07-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{9169B43F-AE90-B84E-BB9B-3E2730E4B499}" name="2025-08-01" totalsRowFunction="custom" dataDxfId="28" totalsRowDxfId="4">
+    <tableColumn id="18" xr3:uid="{9169B43F-AE90-B84E-BB9B-3E2730E4B499}" name="2025-08-01" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
       <totalsRowFormula>SUMIF(jtrn[Movement], "Credit", jtrn[2025-08-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-08-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{16A4B7C1-DCCD-BC42-80A2-5A9B0AFE62B7}" name="2025-09-01" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="3">
+    <tableColumn id="19" xr3:uid="{16A4B7C1-DCCD-BC42-80A2-5A9B0AFE62B7}" name="2025-09-01" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="8">
       <totalsRowFormula>SUMIF(jtrn[Movement], "Credit", jtrn[2025-09-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-09-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{DA0D9353-5004-BC49-A034-377720B302FE}" name="2025-10-01" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="2">
+    <tableColumn id="20" xr3:uid="{DA0D9353-5004-BC49-A034-377720B302FE}" name="2025-10-01" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="6">
       <totalsRowFormula>SUMIF(jtrn[Movement], "Credit", jtrn[2025-10-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-10-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{2CAF52BB-84EF-4B4E-9560-96A6E500A093}" name="2025-11-01" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="1">
+    <tableColumn id="21" xr3:uid="{2CAF52BB-84EF-4B4E-9560-96A6E500A093}" name="2025-11-01" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4">
       <totalsRowFormula>SUMIF(jtrn[Movement], "Credit", jtrn[2025-11-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-11-01])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{2627D4F2-2727-3545-907E-0FB0C0AA352F}" name="2025-12-01" totalsRowFunction="custom" dataDxfId="24" totalsRowDxfId="0">
+    <tableColumn id="22" xr3:uid="{2627D4F2-2727-3545-907E-0FB0C0AA352F}" name="2025-12-01" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="2">
       <totalsRowFormula>SUMIF(jtrn[Movement], "Credit", jtrn[2025-12-01]) - SUMIF(jtrn[Movement], "Debit", jtrn[2025-12-01])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -2244,8 +2244,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AD70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="109" workbookViewId="0">
-      <selection activeCell="S75" sqref="S75"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScale="109" workbookViewId="0">
+      <selection activeCell="T47" sqref="T47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4567,7 +4567,7 @@
       <c r="S46" t="s">
         <v>67</v>
       </c>
-      <c r="T46">
+      <c r="T46" s="42">
         <v>10545.22</v>
       </c>
       <c r="V46" s="42" t="s">
@@ -4594,7 +4594,7 @@
       <c r="S47" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="T47" s="45">
+      <c r="T47" s="42">
         <v>6305</v>
       </c>
       <c r="V47" s="42" t="s">
@@ -4766,10 +4766,10 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="M41:V42">
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>